<commit_message>
Updated EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
</commit_message>
<xml_diff>
--- a/Documents/External/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
+++ b/Documents/External/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnslooten/Documents/Projects/Philips EWS/QMS documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaskvortsova/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2340" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="887" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="887"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -46,6 +46,39 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="D109" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+remove
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="131">
   <si>
@@ -499,7 +532,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +612,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -691,30 +735,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -742,6 +762,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1167,7 +1211,7 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A270" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
@@ -1184,114 +1228,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
@@ -1459,16 +1503,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
@@ -1486,11 +1530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A35" zoomScale="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView view="pageLayout" zoomScale="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1503,1238 +1547,1238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37" t="s">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37" t="s">
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="D36" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37" t="s">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37" t="s">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37" t="s">
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37" t="s">
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37" t="s">
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C52" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="D52" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37" t="s">
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D53" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37" t="s">
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37" t="s">
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="37" t="s">
+      <c r="D55" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37" t="s">
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="37" t="s">
+      <c r="D56" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37" t="s">
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="37" t="s">
+      <c r="D57" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37" t="s">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D58" s="37" t="s">
+      <c r="D58" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37" t="s">
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D59" s="37" t="s">
+      <c r="D59" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="37"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37" t="s">
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="37" t="s">
+      <c r="D60" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37" t="s">
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="37" t="s">
+      <c r="D61" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="37" t="s">
+      <c r="C62" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="37" t="s">
+      <c r="D62" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37" t="s">
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D63" s="37" t="s">
+      <c r="D63" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37" t="s">
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="37" t="s">
+      <c r="D64" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37" t="s">
+      <c r="A65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D65" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A66" s="37"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37" t="s">
+      <c r="A66" s="29"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="37" t="s">
+      <c r="D66" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37" t="s">
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D67" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37" t="s">
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D68" s="37" t="s">
+      <c r="D68" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37" t="s">
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37" t="s">
+      <c r="A70" s="29"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="37" t="s">
+      <c r="D70" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37" t="s">
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D71" s="37" t="s">
+      <c r="D71" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A72" s="37" t="s">
+      <c r="A72" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="37" t="s">
+      <c r="B72" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="37" t="s">
+      <c r="D72" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A73" s="37">
+      <c r="A73" s="29">
         <v>70307</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B73" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="37" t="s">
+      <c r="C73" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D73" s="37" t="s">
+      <c r="D73" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37" t="s">
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D74" s="37" t="s">
+      <c r="D74" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A75" s="37"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37" t="s">
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D75" s="37" t="s">
+      <c r="D75" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A76" s="37"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37" t="s">
+      <c r="A76" s="29"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D76" s="37" t="s">
+      <c r="D76" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A77" s="37"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="37" t="s">
+      <c r="A77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="37" t="s">
+      <c r="D77" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37" t="s">
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D78" s="37" t="s">
+      <c r="D78" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="37"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="37" t="s">
+      <c r="A79" s="29"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37" t="s">
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D80" s="37" t="s">
+      <c r="D80" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37" t="s">
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D81" s="37" t="s">
+      <c r="D81" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="37" t="s">
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D82" s="37" t="s">
+      <c r="D82" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A83" s="37" t="s">
+      <c r="A83" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="37" t="s">
+      <c r="B83" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C83" s="37" t="s">
+      <c r="C83" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="37" t="s">
+      <c r="D83" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="75" x14ac:dyDescent="0.2">
-      <c r="A84" s="37" t="s">
+      <c r="A84" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B84" s="37" t="s">
+      <c r="B84" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C84" s="37" t="s">
+      <c r="C84" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D84" s="37" t="s">
+      <c r="D84" s="29" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B85" s="37" t="s">
+      <c r="B85" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="C85" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="37" t="s">
+      <c r="D85" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A86" s="37" t="s">
+      <c r="A86" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B86" s="37" t="s">
+      <c r="B86" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C86" s="37" t="s">
+      <c r="C86" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="37" t="s">
+      <c r="D86" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A87" s="37" t="s">
+      <c r="A87" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B87" s="37" t="s">
+      <c r="B87" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="37" t="s">
+      <c r="C87" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D87" s="37" t="s">
+      <c r="D87" s="29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A88" s="37" t="s">
+      <c r="A88" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="37" t="s">
+      <c r="B88" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="37" t="s">
+      <c r="C88" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="37" t="s">
+      <c r="D88" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37" t="s">
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="37" t="s">
+      <c r="D89" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37" t="s">
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D90" s="37" t="s">
+      <c r="D90" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37" t="s">
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D91" s="37" t="s">
+      <c r="D91" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37" t="s">
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D92" s="37" t="s">
+      <c r="D92" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A93" s="37"/>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37" t="s">
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D93" s="37" t="s">
+      <c r="D93" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A94" s="37"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37" t="s">
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D94" s="37" t="s">
+      <c r="D94" s="29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A95" s="37"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37" t="s">
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D95" s="37" t="s">
+      <c r="D95" s="29" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="37"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="37" t="s">
+      <c r="A96" s="29"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D96" s="37" t="s">
+      <c r="D96" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="37" t="s">
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D97" s="37" t="s">
+      <c r="D97" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="37"/>
-      <c r="B98" s="37"/>
-      <c r="C98" s="37" t="s">
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D98" s="37" t="s">
+      <c r="D98" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="37" t="s">
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="37" t="s">
+      <c r="D99" s="29" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="37"/>
-      <c r="B100" s="37"/>
-      <c r="C100" s="37" t="s">
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D100" s="37" t="s">
+      <c r="D100" s="29" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A101" s="37" t="s">
+      <c r="A101" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="37" t="s">
+      <c r="B101" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C101" s="37" t="s">
+      <c r="C101" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D101" s="37" t="s">
+      <c r="D101" s="29" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A102" s="37"/>
-      <c r="B102" s="37"/>
-      <c r="C102" s="37" t="s">
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D102" s="37" t="s">
+      <c r="D102" s="29" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A103" s="37" t="s">
+      <c r="A103" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B103" s="37" t="s">
+      <c r="B103" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C103" s="37" t="s">
+      <c r="C103" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D103" s="37" t="s">
+      <c r="D103" s="29" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A104" s="37"/>
-      <c r="B104" s="37"/>
-      <c r="C104" s="37" t="s">
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D104" s="37" t="s">
+      <c r="D104" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A105" s="37" t="s">
+      <c r="A105" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B105" s="37" t="s">
+      <c r="B105" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C105" s="37" t="s">
+      <c r="C105" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D105" s="37" t="s">
+      <c r="D105" s="29" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A106" s="37"/>
-      <c r="B106" s="37"/>
-      <c r="C106" s="37" t="s">
+      <c r="A106" s="29"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D106" s="37" t="s">
+      <c r="D106" s="29" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A107" s="37" t="s">
+      <c r="A107" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="37" t="s">
+      <c r="B107" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="37" t="s">
+      <c r="C107" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D107" s="37" t="s">
+      <c r="D107" s="29" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A108" s="37"/>
-      <c r="B108" s="37"/>
-      <c r="C108" s="37" t="s">
+      <c r="A108" s="29"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D108" s="37" t="s">
+      <c r="D108" s="29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="37" t="s">
+      <c r="B109" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
+      <c r="C109" s="29"/>
+      <c r="D109" s="29"/>
     </row>
     <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A110" s="37" t="s">
+      <c r="A110" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B110" s="37" t="s">
+      <c r="B110" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C110" s="37" t="s">
+      <c r="C110" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="D110" s="37" t="s">
+      <c r="D110" s="29" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A111" s="37" t="s">
+      <c r="A111" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B111" s="37" t="s">
+      <c r="B111" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="C111" s="37" t="s">
+      <c r="C111" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D111" s="37" t="s">
+      <c r="D111" s="29" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B112" s="37" t="s">
+      <c r="B112" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C112" s="37" t="s">
+      <c r="C112" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D112" s="37" t="s">
+      <c r="D112" s="29" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A113" s="37" t="s">
+      <c r="A113" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B113" s="37" t="s">
+      <c r="B113" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C113" s="37" t="s">
+      <c r="C113" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D113" s="37" t="s">
+      <c r="D113" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="37"/>
-      <c r="B114" s="37"/>
-      <c r="C114" s="37" t="s">
+      <c r="A114" s="29"/>
+      <c r="B114" s="29"/>
+      <c r="C114" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D114" s="37" t="s">
+      <c r="D114" s="29" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2746,6 +2790,7 @@
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;20&amp;K04+000Requirement Traceability Matrix - Easy Wi-Fi Setup UX</oddHeader>
     <oddFooter>&amp;L&amp;12Doc ID: EWS000003_x000D_Version: 0.1_x000D_Status: &lt; Approved&gt;_x000D_&amp;CDocument Title:   _x000D_Requirements Traceability Matrix - Easy Wi-Fi Setup UX  _x000D_Content  based on:_x000D_Template ID: CDPP-T-03000003 Template Version: 1.0&amp;RAuthor: Lynn Slooten_x000D_Approver: Thijs Winter_x000D_</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -2759,7 +2804,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A95" zoomScale="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2774,13 +2819,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
@@ -2799,20 +2844,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="32">
         <v>43055</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="31" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2824,20 +2869,20 @@
       <c r="E5" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.15">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="6"/>
@@ -2860,10 +2905,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="33" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="7"/>
@@ -2958,12 +3003,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8C356F8E1D36642B88ADD05DBA2175B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5caac0f2500184a09392517ffd772eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3077,7 +3116,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3086,22 +3125,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8F17C31-F114-41DE-B3DD-D74FBD45A200}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3117,10 +3147,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>